<commit_message>
EPI 11.10 + Yandex. Search in a sorted 2D-array m*n
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -11,7 +11,7 @@
     <sheet name="Списки" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>11.9 Computing square roots</t>
-  </si>
-  <si>
-    <t>11.10 2D array search</t>
   </si>
   <si>
     <t>11.11 Finding the winner and runner-up</t>
@@ -826,12 +823,15 @@
   <si>
     <t>8.9 Printing a BST in level-order (BFS)</t>
   </si>
+  <si>
+    <t>11.10 2D sorted array search</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,6 +867,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -959,7 +967,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -996,18 +1004,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1020,9 +1029,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1060,7 +1069,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1132,7 +1141,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1333,33 +1342,33 @@
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="F1" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="F2" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1372,10 +1381,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1383,10 +1392,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1394,10 +1403,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,7 +1415,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1414,10 +1423,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,10 +1434,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1436,10 +1445,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,10 +1456,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,7 +1467,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1476,10 +1485,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1495,7 +1504,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,10 +1531,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,7 +1552,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1573,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1595,12 +1604,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1620,7 +1629,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,7 +1647,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,7 +1656,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1663,7 +1672,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,7 +1686,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,7 +1695,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1711,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1711,7 +1720,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1721,8 +1730,8 @@
       <c r="C43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="24" t="s">
-        <v>248</v>
+      <c r="D43" s="22" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,7 +1745,7 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,7 +1754,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1754,7 +1763,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1763,7 +1772,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1772,7 +1781,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,7 +1790,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,7 +1799,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,7 +1808,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,7 +1817,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1826,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1837,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,7 +1848,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,7 +1867,7 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1867,7 +1876,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,7 +1885,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,7 +1894,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1894,7 +1903,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,7 +1912,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1928,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1929,11 +1938,11 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,7 +1951,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,7 +1967,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1978,7 +1987,7 @@
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,7 +2008,7 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +2031,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,7 +2040,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,7 +2049,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,7 +2058,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2067,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,7 +2092,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +2101,7 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,7 +2112,7 @@
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,7 +2126,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,7 +2135,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,15 +2144,15 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C93" s="3"/>
-      <c r="D93" s="25"/>
+      <c r="D93" s="23"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
@@ -2151,7 +2160,7 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2160,7 +2169,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2171,7 +2180,7 @@
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2180,7 +2189,7 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2191,7 +2200,7 @@
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,7 +2219,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2219,7 +2228,7 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,16 +2237,16 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,7 +2264,7 @@
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,7 +2282,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,51 +2298,51 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>107</v>
+        <v>261</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D111" s="3"/>
+      <c r="D111" s="26"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>19</v>
@@ -2342,23 +2351,23 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>21</v>
@@ -2367,14 +2376,14 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>19</v>
@@ -2383,37 +2392,37 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>21</v>
@@ -2422,16 +2431,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>21</v>
@@ -2440,34 +2449,34 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>19</v>
@@ -2476,7 +2485,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>19</v>
@@ -2485,23 +2494,23 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>19</v>
@@ -2510,7 +2519,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>19</v>
@@ -2519,89 +2528,89 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>19</v>
@@ -2610,50 +2619,50 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>21</v>
@@ -2662,33 +2671,33 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>19</v>
@@ -2697,43 +2706,43 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>19</v>
@@ -2742,7 +2751,7 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -2751,7 +2760,7 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>21</v>
@@ -2760,66 +2769,66 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>19</v>
@@ -2828,7 +2837,7 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>19</v>
@@ -2837,7 +2846,7 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2846,47 +2855,47 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>21</v>
@@ -2895,18 +2904,18 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
@@ -2915,58 +2924,56 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="E189" s="20" t="s">
-        <v>253</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>19</v>
@@ -2975,19 +2982,19 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D192" s="19"/>
       <c r="E192" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="193" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
@@ -2996,7 +3003,7 @@
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
@@ -3005,96 +3012,96 @@
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C195" s="3"/>
       <c r="D195" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="196" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E196" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
     </row>
     <row r="199" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="200" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E200" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="201" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
     <row r="202" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
       <c r="E203" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="204" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>21</v>
@@ -3103,12 +3110,12 @@
     </row>
     <row r="206" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B206" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="207" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>19</v>
@@ -3117,16 +3124,16 @@
     </row>
     <row r="208" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C208" s="3"/>
       <c r="D208" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>21</v>
@@ -3135,7 +3142,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>21</v>
@@ -3144,45 +3151,45 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>19</v>
@@ -3191,26 +3198,26 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B217" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C218" s="3"/>
       <c r="D218" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>19</v>
@@ -3219,16 +3226,16 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C220" s="3"/>
       <c r="D220" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>21</v>
@@ -3237,204 +3244,207 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C225" s="3"/>
       <c r="D225" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C227" s="3"/>
       <c r="D227" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B230" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C229" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B230" s="3" t="s">
+      <c r="C230" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B231" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D230" s="3"/>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B231" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B233" s="3" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B233" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E234" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B237" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B237" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D238" s="3"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C239" s="3"/>
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>19</v>
@@ -3473,22 +3483,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Yandex. Longest Common Subsequence (LCSS)
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="263">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>11.10 2D sorted array search</t>
+  </si>
+  <si>
+    <t>15.x Longest Common Subsequence (LCSS)</t>
   </si>
 </sst>
 </file>
@@ -1006,13 +1009,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1315,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L245"/>
+  <dimension ref="A1:L246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,11 +1345,11 @@
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
         <v>238</v>
       </c>
@@ -1357,11 +1360,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
         <v>239</v>
       </c>
@@ -2308,7 +2311,7 @@
       <c r="C111" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D111" s="26"/>
+      <c r="D111" s="24"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
@@ -2684,7 +2687,7 @@
         <v>151</v>
       </c>
       <c r="C157" s="3"/>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="14" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2973,37 +2976,37 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D192" s="19"/>
-      <c r="E192" t="s">
-        <v>252</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D192" s="14"/>
     </row>
     <row r="193" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>182</v>
+        <v>258</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D193" s="3"/>
+      <c r="D193" s="19"/>
+      <c r="E193" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
@@ -3012,137 +3015,137 @@
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C195" s="3"/>
-      <c r="D195" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D195" s="3"/>
     </row>
     <row r="196" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E196" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>253</v>
+        <v>185</v>
       </c>
       <c r="C197" s="3"/>
-      <c r="D197" s="14" t="s">
-        <v>245</v>
+      <c r="D197" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E197" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>186</v>
+        <v>253</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
+      <c r="D198" s="14" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="199" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="3" t="s">
-        <v>247</v>
-      </c>
+      <c r="D199" s="3"/>
     </row>
     <row r="200" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E200" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="201" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
+      <c r="D201" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E201" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="202" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
-      <c r="E203" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="204" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
+      <c r="E204" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B206" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C205" s="3" t="s">
+      <c r="C206" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D205" s="3"/>
-    </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B206" s="9" t="s">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B207" s="9" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D207" s="3"/>
     </row>
     <row r="208" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C208" s="3"/>
-      <c r="D208" s="3" t="s">
-        <v>244</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D209" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="C209" s="3"/>
+      <c r="D209" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>21</v>
@@ -3151,305 +3154,314 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>247</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C212" s="3"/>
+        <v>199</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D212" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C213" s="3"/>
       <c r="D213" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
+        <v>201</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C215" s="3"/>
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B216" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C215" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D215" s="3"/>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="7" t="s">
+      <c r="C216" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B217" s="9" t="s">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="9" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D219" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="C219" s="3"/>
+      <c r="D219" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3" t="s">
-        <v>245</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D221" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B224" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B224" s="9" t="s">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B225" s="9" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B225" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C225" s="3"/>
-      <c r="D225" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C226" s="3"/>
-      <c r="D226" s="3"/>
+      <c r="D226" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C227" s="3"/>
-      <c r="D227" s="3" t="s">
-        <v>246</v>
-      </c>
+      <c r="D227" s="3"/>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D230" s="3"/>
+      <c r="D230" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B232" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C231" s="3"/>
-      <c r="D231" s="3" t="s">
+      <c r="C232" s="3"/>
+      <c r="D232" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" s="7" t="s">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="7" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B233" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E234" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
+      </c>
+      <c r="E235" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C237" s="3"/>
-      <c r="D237" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C238" s="3"/>
       <c r="D238" s="3"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C239" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D239" s="3"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C240" s="3"/>
-      <c r="D240" s="3" t="s">
-        <v>244</v>
-      </c>
+      <c r="D240" s="3"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C245" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D245" s="3"/>
+      <c r="C246" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D246" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changes in comments and EPI plan
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>17.1 Ties in a presidential election</t>
-  </si>
-  <si>
-    <t>17.2 The knapsack problem</t>
   </si>
   <si>
     <t>17.3 Dividing the spoils</t>
@@ -827,7 +824,10 @@
     <t>11.10 2D sorted array search</t>
   </si>
   <si>
-    <t>15.x Longest Common Subsequence (LCSS)</t>
+    <t>17.2 The 0-1 knapsack problem</t>
+  </si>
+  <si>
+    <t>15.5.3 Longest common subsequence (LCSS)</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,32 +1346,32 @@
         <v>22</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1384,10 +1384,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1395,10 +1395,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1437,10 +1437,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1448,10 +1448,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1459,10 +1459,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1488,10 +1488,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1534,10 +1534,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1607,12 +1607,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,11 +1941,11 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,7 +2043,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,12 +2147,12 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="23"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,16 +2240,16 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,12 +2301,12 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,7 +2660,7 @@
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
@@ -2776,16 +2776,16 @@
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -2931,7 +2931,7 @@
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -2941,37 +2941,37 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -2979,13 +2979,13 @@
         <v>262</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>19</v>
@@ -2994,14 +2994,14 @@
     </row>
     <row r="193" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D193" s="19"/>
       <c r="E193" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.25">
@@ -3037,19 +3037,19 @@
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E197" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="199" spans="2:5" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="201" spans="2:5" x14ac:dyDescent="0.25">
@@ -3074,10 +3074,10 @@
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E201" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="202" spans="2:5" x14ac:dyDescent="0.25">
@@ -3101,7 +3101,7 @@
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
       <c r="E204" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="C209" s="3"/>
       <c r="D209" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
         <v>19</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="C213" s="3"/>
       <c r="D213" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
         <v>19</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="C219" s="3"/>
       <c r="D219" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="C221" s="3"/>
       <c r="D221" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>19</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -3351,51 +3351,51 @@
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E235" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>21</v>
@@ -3404,59 +3404,59 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>19</v>
@@ -3495,22 +3495,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving all combinatorial problems to C++, part 1
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="262">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -769,9 +769,6 @@
   </si>
   <si>
     <t>14.12 Traversal orders in BST</t>
-  </si>
-  <si>
-    <t>!</t>
   </si>
   <si>
     <r>
@@ -821,13 +818,13 @@
     <t>8.9 Printing a BST in level-order (BFS)</t>
   </si>
   <si>
-    <t>11.10 2D sorted array search</t>
-  </si>
-  <si>
     <t>17.2 The 0-1 knapsack problem</t>
   </si>
   <si>
     <t>15.5.3 Longest common subsequence (LCSS)</t>
+  </si>
+  <si>
+    <t>11.10 Search in a sorted matrix</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1573,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
@@ -2306,7 +2303,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
@@ -2941,7 +2938,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>240</v>
@@ -2952,7 +2949,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>240</v>
@@ -2965,7 +2962,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>240</v>
@@ -2976,7 +2973,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>240</v>
@@ -2985,26 +2982,23 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D192" s="14"/>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D193" s="19"/>
-      <c r="E193" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>182</v>
       </c>
@@ -3013,7 +3007,7 @@
       </c>
       <c r="D194" s="3"/>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>183</v>
       </c>
@@ -3022,7 +3016,7 @@
       </c>
       <c r="D195" s="3"/>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>184</v>
       </c>
@@ -3031,7 +3025,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>185</v>
       </c>
@@ -3039,27 +3033,24 @@
       <c r="D197" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E197" t="s">
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="3" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B198" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
         <v>187</v>
       </c>
@@ -3068,7 +3059,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
         <v>188</v>
       </c>
@@ -3076,42 +3067,36 @@
       <c r="D201" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E201" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
         <v>189</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
         <v>191</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
-      <c r="E204" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
         <v>193</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
         <v>192</v>
       </c>
@@ -3120,12 +3105,12 @@
       </c>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
         <v>195</v>
       </c>
@@ -3272,12 +3257,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B225" s="9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
         <v>214</v>
       </c>
@@ -3286,14 +3271,14 @@
         <v>243</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
         <v>215</v>
       </c>
       <c r="C227" s="3"/>
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
         <v>216</v>
       </c>
@@ -3302,7 +3287,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
         <v>217</v>
       </c>
@@ -3311,7 +3296,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
         <v>218</v>
       </c>
@@ -3322,7 +3307,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
         <v>219</v>
       </c>
@@ -3331,7 +3316,7 @@
       </c>
       <c r="D231" s="3"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
         <v>220</v>
       </c>
@@ -3340,12 +3325,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
         <v>222</v>
       </c>
@@ -3354,19 +3339,16 @@
         <v>245</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E235" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
         <v>223</v>
       </c>
@@ -3375,7 +3357,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
         <v>224</v>
       </c>
@@ -3386,14 +3368,14 @@
         <v>244</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
         <v>225</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
         <v>226</v>
       </c>
@@ -3402,7 +3384,7 @@
       </c>
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
Added DP solution for SSS.
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="263">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>11.10 Search in a sorted matrix</t>
+  </si>
+  <si>
+    <t>17.0 Subset sum (SSS)</t>
   </si>
 </sst>
 </file>
@@ -967,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1013,10 +1016,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1029,9 +1033,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1069,7 +1073,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1141,7 +1145,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1315,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L246"/>
+  <dimension ref="A1:L247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="E234" sqref="E234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3331,119 +3335,131 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="27"/>
       <c r="B234" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3" t="s">
-        <v>245</v>
+        <v>262</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D234" s="14" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C237" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="C237" s="3"/>
       <c r="D237" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C238" s="3"/>
-      <c r="D238" s="3"/>
+        <v>224</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="C239" s="3"/>
       <c r="D239" s="3"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C240" s="3"/>
+        <v>226</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D240" s="3"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C241" s="3"/>
-      <c r="D241" s="3" t="s">
-        <v>243</v>
-      </c>
+      <c r="D241" s="3"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C246" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D246" s="3"/>
+      <c r="C247" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D247" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added searching for single SSA
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -1010,17 +1010,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1033,9 +1033,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1073,7 +1073,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1145,7 +1145,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1321,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="E234" sqref="E234"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,11 +1346,11 @@
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="15" t="s">
         <v>237</v>
       </c>
@@ -1361,11 +1361,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="16" t="s">
         <v>238</v>
       </c>
@@ -3335,7 +3335,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="27"/>
+      <c r="A234" s="25"/>
       <c r="B234" s="3" t="s">
         <v>262</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>259</v>
       </c>
       <c r="C236" s="3"/>
-      <c r="D236" s="3" t="s">
+      <c r="D236" s="18" t="s">
         <v>243</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated some docs, headers and projects
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -11,12 +11,12 @@
     <sheet name="Списки" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="263">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>11.9 Computing square roots</t>
+  </si>
+  <si>
+    <t>11.10 2D array search</t>
   </si>
   <si>
     <t>11.11 Finding the winner and runner-up</t>
@@ -818,23 +821,20 @@
     <t>8.9 Printing a BST in level-order (BFS)</t>
   </si>
   <si>
-    <t>17.2 The 0-1 knapsack problem</t>
-  </si>
-  <si>
-    <t>15.5.3 Longest common subsequence (LCSS)</t>
-  </si>
-  <si>
-    <t>11.10 Search in a sorted matrix</t>
-  </si>
-  <si>
-    <t>17.0 Subset sum (SSS)</t>
+    <t>17.2.1 The knapsack 0-1 problem (KS01)</t>
+  </si>
+  <si>
+    <t>17.2.2 The knapsack 0-1 problem with repeatitions (KSU)</t>
+  </si>
+  <si>
+    <t>17.2.3 The fractional knapsack problem (KSF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -870,14 +870,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -970,7 +962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1009,8 +1001,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1019,8 +1010,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1033,9 +1024,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1073,7 +1064,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1145,7 +1136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1321,7 +1312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
       <selection activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
@@ -1346,33 +1337,33 @@
       <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="F1" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="F2" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,10 +1376,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1396,10 +1387,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1407,10 +1398,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1419,7 +1410,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1427,10 +1418,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1438,10 +1429,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1449,10 +1440,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1460,10 +1451,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1489,10 +1480,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1508,7 +1499,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,10 +1526,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,7 +1547,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,7 +1568,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1608,12 +1599,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1633,7 +1624,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,7 +1642,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,7 +1651,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,7 +1667,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,7 +1681,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,7 +1690,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,7 +1706,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1724,7 +1715,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1735,7 +1726,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1749,7 +1740,7 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1749,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,7 +1758,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,7 +1767,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1785,7 +1776,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,7 +1785,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,7 +1794,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +1803,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,7 +1812,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1830,7 +1821,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,7 +1832,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1852,7 +1843,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,7 +1862,7 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,7 +1871,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1889,7 +1880,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,7 +1889,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,7 +1898,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1907,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,7 +1923,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,11 +1933,11 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +1946,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,7 +1962,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1991,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,7 +2003,7 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2035,7 +2026,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,7 +2035,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2044,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2062,7 +2053,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2071,7 +2062,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,7 +2087,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,7 +2096,7 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,7 +2107,7 @@
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,7 +2121,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2130,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,12 +2139,12 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="23"/>
@@ -2164,7 +2155,7 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,7 +2164,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,7 +2175,7 @@
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2193,7 +2184,7 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2204,7 +2195,7 @@
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2223,7 +2214,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,7 +2223,7 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,16 +2232,16 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,7 +2259,7 @@
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2286,7 +2277,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2302,51 +2293,51 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>261</v>
+        <v>107</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D111" s="24"/>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>19</v>
@@ -2355,23 +2346,23 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>21</v>
@@ -2380,14 +2371,14 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>19</v>
@@ -2396,37 +2387,37 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>21</v>
@@ -2435,16 +2426,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>21</v>
@@ -2453,34 +2444,34 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>19</v>
@@ -2489,7 +2480,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>19</v>
@@ -2498,23 +2489,23 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>19</v>
@@ -2523,7 +2514,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>19</v>
@@ -2532,89 +2523,89 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>19</v>
@@ -2623,50 +2614,50 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>21</v>
@@ -2675,33 +2666,33 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C157" s="3"/>
-      <c r="D157" s="14" t="s">
-        <v>243</v>
+      <c r="D157" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>19</v>
@@ -2710,43 +2701,43 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>19</v>
@@ -2755,7 +2746,7 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -2764,7 +2755,7 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>21</v>
@@ -2773,66 +2764,66 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>19</v>
@@ -2841,7 +2832,7 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>19</v>
@@ -2850,7 +2841,7 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2859,47 +2850,47 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>21</v>
@@ -2908,18 +2899,18 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
@@ -2928,83 +2919,83 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>240</v>
+        <v>19</v>
       </c>
       <c r="D191" s="14"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D192" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="D192" s="19"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>256</v>
+        <v>183</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D193" s="19"/>
+      <c r="D193" s="3"/>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
@@ -3013,50 +3004,50 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D195" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>185</v>
+        <v>252</v>
       </c>
       <c r="C197" s="3"/>
-      <c r="D197" s="3" t="s">
-        <v>243</v>
+      <c r="D197" s="14" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>251</v>
+        <v>187</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="14" t="s">
-        <v>244</v>
-      </c>
+      <c r="D198" s="3"/>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
+      <c r="D199" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
@@ -3065,30 +3056,28 @@
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="D201" s="3" t="s">
-        <v>245</v>
-      </c>
+      <c r="D201" s="3"/>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
@@ -3097,44 +3086,46 @@
       <c r="B205" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C205" s="3"/>
+      <c r="C205" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D206" s="3"/>
+      <c r="B206" s="9" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="9" t="s">
-        <v>194</v>
-      </c>
+      <c r="B207" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D207" s="3"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D208" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="C208" s="3"/>
+      <c r="D208" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C209" s="3"/>
-      <c r="D209" s="3" t="s">
-        <v>243</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D209" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>21</v>
@@ -3143,109 +3134,109 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D211" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C212" s="3"/>
       <c r="D212" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C213" s="3"/>
+        <v>202</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D213" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D214" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C214" s="3"/>
+      <c r="D214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C215" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D215" s="3"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B216" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D216" s="3"/>
+      <c r="A216" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="7" t="s">
-        <v>204</v>
+      <c r="B217" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="9" t="s">
-        <v>211</v>
+      <c r="B218" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3" t="s">
-        <v>243</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D219" s="3"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D220" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3" t="s">
-        <v>244</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D221" s="3"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D222" s="3"/>
+        <v>210</v>
+      </c>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="3" t="s">
@@ -3253,147 +3244,144 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B224" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C224" s="3"/>
-      <c r="D224" s="3" t="s">
-        <v>244</v>
+      <c r="B224" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="9" t="s">
-        <v>212</v>
+      <c r="B225" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C225" s="3"/>
+      <c r="D225" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C226" s="3"/>
-      <c r="D226" s="3" t="s">
-        <v>243</v>
-      </c>
+      <c r="D226" s="3"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C227" s="3"/>
-      <c r="D227" s="3"/>
+      <c r="D227" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C229" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D229" s="3" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D230" s="3" t="s">
-        <v>246</v>
-      </c>
+      <c r="D230" s="3"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D231" s="3"/>
+        <v>221</v>
+      </c>
+      <c r="C231" s="3"/>
+      <c r="D231" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B232" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C232" s="3"/>
-      <c r="D232" s="3" t="s">
+      <c r="A232" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B233" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="25"/>
       <c r="B234" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="C234" s="3"/>
       <c r="D234" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="C235" s="3"/>
-      <c r="D235" s="3" t="s">
-        <v>245</v>
+      <c r="D235" s="14" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C236" s="3"/>
-      <c r="D236" s="18" t="s">
-        <v>243</v>
+      <c r="D236" s="24" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C239" s="3"/>
       <c r="D239" s="3"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>21</v>
@@ -3402,59 +3390,59 @@
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>19</v>
@@ -3493,22 +3481,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPI Plan, task updates
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="264">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -84,9 +84,6 @@
     <t>*****</t>
   </si>
   <si>
-    <t>Статус</t>
-  </si>
-  <si>
     <t>6.3 Max difference</t>
   </si>
   <si>
@@ -574,9 +571,6 @@
   </si>
   <si>
     <t>15.10 Searching for a sequence in a 2D array</t>
-  </si>
-  <si>
-    <t>15.11 Levenshtein distances</t>
   </si>
   <si>
     <t>15.13 Pretty printing</t>
@@ -828,6 +822,15 @@
   </si>
   <si>
     <t>17.2.3 The fractional knapsack problem (KSF)</t>
+  </si>
+  <si>
+    <t>15.5.3 Longest Common Subsequence (LCSS)</t>
+  </si>
+  <si>
+    <t>15.11 Levenshtein distance</t>
+  </si>
+  <si>
+    <t>Приоритет</t>
   </si>
 </sst>
 </file>
@@ -962,7 +965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1002,6 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1310,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L247"/>
+  <dimension ref="A1:L248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="E236" sqref="E236"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,35 +1339,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="15" t="s">
-        <v>238</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="16" t="s">
-        <v>239</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1376,10 +1380,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1387,10 +1391,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1398,10 +1402,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1410,7 +1414,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1418,10 +1422,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1429,10 +1433,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1440,10 +1444,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1451,10 +1455,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1462,7 +1466,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1480,10 +1484,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1499,7 +1503,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1522,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,10 +1530,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,23 +1547,23 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>19</v>
@@ -1568,7 +1572,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1577,7 +1581,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>19</v>
@@ -1586,7 +1590,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>21</v>
@@ -1595,16 +1599,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1613,23 +1617,23 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>19</v>
@@ -1638,336 +1642,336 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="18"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>19</v>
@@ -1976,98 +1980,98 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>19</v>
@@ -2076,131 +2080,131 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="18"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="23"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>21</v>
@@ -2209,44 +2213,44 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>19</v>
@@ -2255,16 +2259,16 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>19</v>
@@ -2273,32 +2277,32 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
@@ -2307,37 +2311,37 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>19</v>
@@ -2346,23 +2350,23 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>21</v>
@@ -2371,14 +2375,14 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>19</v>
@@ -2387,37 +2391,37 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>21</v>
@@ -2426,16 +2430,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>21</v>
@@ -2444,34 +2448,34 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>19</v>
@@ -2480,7 +2484,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>19</v>
@@ -2489,23 +2493,23 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>19</v>
@@ -2514,7 +2518,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>19</v>
@@ -2523,89 +2527,89 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>19</v>
@@ -2614,50 +2618,50 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>21</v>
@@ -2666,33 +2670,33 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>19</v>
@@ -2701,43 +2705,43 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>19</v>
@@ -2746,7 +2750,7 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -2755,7 +2759,7 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>21</v>
@@ -2764,66 +2768,66 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>19</v>
@@ -2832,7 +2836,7 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>19</v>
@@ -2841,7 +2845,7 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2850,47 +2854,47 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>21</v>
@@ -2899,18 +2903,18 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
@@ -2919,83 +2923,85 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>244</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="C190" s="3"/>
+      <c r="D190" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E190" s="25"/>
+      <c r="F190" s="21"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D191" s="14"/>
+        <v>239</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D192" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="D192" s="14"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D193" s="3"/>
+      <c r="D193" s="19"/>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
@@ -3004,16 +3010,16 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C195" s="3"/>
-      <c r="D195" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D195" s="3"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
@@ -3022,110 +3028,110 @@
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C197" s="3"/>
-      <c r="D197" s="14" t="s">
-        <v>245</v>
+      <c r="D197" s="17" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>187</v>
+        <v>250</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
+      <c r="D198" s="14" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="3" t="s">
-        <v>247</v>
-      </c>
+      <c r="D199" s="3"/>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
+      <c r="D201" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B206" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C205" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D205" s="3"/>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D207" s="3"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C208" s="3"/>
-      <c r="D208" s="3" t="s">
-        <v>244</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D209" s="3"/>
+        <v>195</v>
+      </c>
+      <c r="C209" s="3"/>
+      <c r="D209" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>21</v>
@@ -3134,148 +3140,148 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>247</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C212" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D212" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="C213" s="3"/>
       <c r="D213" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C215" s="3"/>
       <c r="D215" s="3"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="7" t="s">
-        <v>205</v>
-      </c>
+      <c r="B216" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D216" s="3"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B217" s="9" t="s">
-        <v>212</v>
+      <c r="A217" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3" t="s">
-        <v>244</v>
+      <c r="B218" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D219" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="C219" s="3"/>
+      <c r="D219" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3" t="s">
-        <v>245</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D221" s="3"/>
+        <v>206</v>
+      </c>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B224" s="9" t="s">
-        <v>213</v>
+      <c r="B224" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C225" s="3"/>
-      <c r="D225" s="3" t="s">
-        <v>244</v>
+      <c r="B225" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C226" s="3"/>
-      <c r="D226" s="3"/>
+      <c r="D226" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C227" s="3"/>
-      <c r="D227" s="3" t="s">
-        <v>246</v>
-      </c>
+      <c r="D227" s="3"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
@@ -3284,170 +3290,179 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D230" s="3"/>
+      <c r="D230" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C231" s="3"/>
-      <c r="D231" s="3" t="s">
-        <v>247</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D231" s="3"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="7" t="s">
-        <v>222</v>
+      <c r="B232" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C232" s="3"/>
+      <c r="D232" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B233" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3" t="s">
-        <v>246</v>
+      <c r="A233" s="7" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="C234" s="3"/>
-      <c r="D234" s="14" t="s">
+      <c r="D234" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C236" s="3"/>
-      <c r="D236" s="24" t="s">
-        <v>245</v>
+      <c r="D236" s="14" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="C237" s="3"/>
-      <c r="D237" s="3" t="s">
-        <v>247</v>
+      <c r="D237" s="24" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C238" s="3"/>
       <c r="D238" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C239" s="3"/>
-      <c r="D239" s="3"/>
+        <v>223</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C240" s="3"/>
       <c r="D240" s="3"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C241" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D241" s="3"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C242" s="3"/>
-      <c r="D242" s="3" t="s">
-        <v>244</v>
-      </c>
+      <c r="D242" s="3"/>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D247" s="3"/>
+        <v>231</v>
+      </c>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D248" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3463,7 +3478,7 @@
           <x14:formula1>
             <xm:f>Списки!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3481,22 +3496,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated comments and EPI plan
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="265">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -601,9 +601,6 @@
   </si>
   <si>
     <t>15.21 Minimize waiting time</t>
-  </si>
-  <si>
-    <t>15.22 Scheduling tutors</t>
   </si>
   <si>
     <t>15.23 Job assignment</t>
@@ -831,6 +828,12 @@
   </si>
   <si>
     <t>Приоритет</t>
+  </si>
+  <si>
+    <t>15.22.2 Coin change</t>
+  </si>
+  <si>
+    <t>15.22.1 Scheduling tutors</t>
   </si>
 </sst>
 </file>
@@ -1314,9 +1317,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L248"/>
+  <dimension ref="A1:L249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
       <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
@@ -1339,35 +1342,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
       <c r="I1" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1380,10 +1383,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1391,10 +1394,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1402,10 +1405,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1414,7 +1417,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1422,10 +1425,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1433,10 +1436,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1444,10 +1447,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1455,10 +1458,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1466,7 +1469,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1484,10 +1487,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1503,7 +1506,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1530,10 +1533,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,7 +1554,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1572,7 +1575,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1603,12 +1606,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1628,7 +1631,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,7 +1649,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1655,7 +1658,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1674,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,7 +1688,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,7 +1697,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1713,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1719,7 +1722,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1744,7 +1747,7 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,7 +1756,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,7 +1765,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,7 +1774,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,7 +1783,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,7 +1792,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1801,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,7 +1810,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1816,7 +1819,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,7 +1828,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,7 +1839,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,7 +1850,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1869,7 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1875,7 +1878,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,7 +1887,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,7 +1896,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,7 +1905,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,7 +1914,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1930,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,11 +1940,11 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1950,7 +1953,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +1969,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +1989,7 @@
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2007,7 +2010,7 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2030,7 +2033,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,7 +2042,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2048,7 +2051,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,7 +2060,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2066,7 +2069,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,7 +2094,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2100,7 +2103,7 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2114,7 @@
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,7 +2128,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +2137,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,12 +2146,12 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="23"/>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,7 +2171,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,7 +2182,7 @@
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2188,7 +2191,7 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,7 +2230,7 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,16 +2239,16 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2263,7 +2266,7 @@
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2281,7 +2284,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2297,7 +2300,7 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,7 +2330,7 @@
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2336,7 +2339,7 @@
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2357,7 @@
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2400,7 +2403,7 @@
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2409,7 +2412,7 @@
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,7 +2437,7 @@
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2452,7 +2455,7 @@
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2461,7 +2464,7 @@
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2470,7 +2473,7 @@
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,7 +2507,7 @@
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2531,7 +2534,7 @@
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2545,7 +2548,7 @@
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2554,7 +2557,7 @@
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,16 +2580,16 @@
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2595,7 +2598,7 @@
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,7 +2607,7 @@
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2622,7 +2625,7 @@
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2638,7 +2641,7 @@
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,7 +2659,7 @@
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2684,7 +2687,7 @@
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2709,7 +2712,7 @@
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
@@ -2718,7 +2721,7 @@
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
@@ -2727,7 +2730,7 @@
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
@@ -2736,7 +2739,7 @@
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
@@ -2772,16 +2775,16 @@
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
@@ -2790,7 +2793,7 @@
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
@@ -2813,7 +2816,7 @@
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
@@ -2822,7 +2825,7 @@
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
@@ -2863,7 +2866,7 @@
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -2872,7 +2875,7 @@
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -2909,7 +2912,7 @@
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -2927,7 +2930,7 @@
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -2937,53 +2940,53 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C190" s="3"/>
       <c r="D190" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E190" s="25"/>
       <c r="F190" s="21"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>19</v>
@@ -2992,7 +2995,7 @@
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
@@ -3023,25 +3026,25 @@
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
@@ -3057,7 +3060,7 @@
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
@@ -3066,7 +3069,7 @@
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
@@ -3122,25 +3125,25 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>195</v>
+        <v>264</v>
       </c>
       <c r="C209" s="3"/>
       <c r="D209" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D210" s="3"/>
+        <v>263</v>
+      </c>
+      <c r="C210" s="3"/>
+      <c r="D210" s="14" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>21</v>
@@ -3149,109 +3152,109 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>245</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D212" s="3"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C213" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D213" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C214" s="3"/>
       <c r="D214" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C215" s="3"/>
-      <c r="D215" s="3"/>
+        <v>199</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C216" s="3"/>
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C216" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D216" s="3"/>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="9" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3" t="s">
-        <v>242</v>
+      <c r="B219" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D220" s="3"/>
+        <v>203</v>
+      </c>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3" t="s">
-        <v>243</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D221" s="3"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D222" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3" t="s">
-        <v>244</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="3" t="s">
@@ -3259,178 +3262,178 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="9" t="s">
-        <v>211</v>
+      <c r="B225" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C225" s="3"/>
+      <c r="D225" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C226" s="3"/>
-      <c r="D226" s="3" t="s">
-        <v>242</v>
+      <c r="B226" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C227" s="3"/>
-      <c r="D227" s="3"/>
+      <c r="D227" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C228" s="3"/>
-      <c r="D228" s="3" t="s">
-        <v>244</v>
-      </c>
+      <c r="D228" s="3"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="C230" s="3"/>
       <c r="D230" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D231" s="3"/>
+      <c r="D231" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B233" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="C232" s="3"/>
-      <c r="D232" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B234" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="C235" s="3"/>
-      <c r="D235" s="14" t="s">
-        <v>242</v>
+      <c r="D235" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C237" s="3"/>
-      <c r="D237" s="24" t="s">
-        <v>243</v>
+      <c r="D237" s="14" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>222</v>
+        <v>259</v>
       </c>
       <c r="C238" s="3"/>
-      <c r="D238" s="3" t="s">
-        <v>245</v>
+      <c r="D238" s="24" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C239" s="3"/>
       <c r="D239" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C240" s="3"/>
-      <c r="D240" s="3"/>
+        <v>222</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="C241" s="3"/>
       <c r="D241" s="3"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C242" s="3"/>
+        <v>224</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D242" s="3"/>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C243" s="3"/>
-      <c r="D243" s="3" t="s">
-        <v>242</v>
-      </c>
+      <c r="D243" s="3"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
@@ -3439,30 +3442,39 @@
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D248" s="3"/>
+        <v>230</v>
+      </c>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B249" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D249" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3496,22 +3508,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added EPI 15.26, Huffman Coding
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+      <selection activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,7 +3175,7 @@
         <v>198</v>
       </c>
       <c r="C214" s="3"/>
-      <c r="D214" s="3" t="s">
+      <c r="D214" s="14" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 6.22, phone number mnemonic combinations
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -1017,8 +1017,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1031,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1071,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1143,7 +1143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E214" sqref="E214"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1721,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="14" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 6.14, Sudoku checker, part 2
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -1017,8 +1017,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1031,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1071,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1143,7 +1143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1648,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="14" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 6.3, max difference
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1553,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="14" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 6.15, printing matrix in spiral order
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -11,7 +11,7 @@
     <sheet name="Списки" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -267,12 +267,6 @@
     <t>9.10 The exterior of a binary tree</t>
   </si>
   <si>
-    <t>9.11 Lowest common ancestor</t>
-  </si>
-  <si>
-    <t>9.12 Lowest common ancestor with parent pointer</t>
-  </si>
-  <si>
     <t xml:space="preserve">9.13 Lowest common ancestor, close ancestor </t>
   </si>
   <si>
@@ -502,9 +496,6 @@
   </si>
   <si>
     <t>14.11 Find the k largest elements in a BST</t>
-  </si>
-  <si>
-    <t>14.13 Lowest common ancestor</t>
   </si>
   <si>
     <t>14.14 Descendant and ancestor</t>
@@ -834,6 +825,15 @@
   </si>
   <si>
     <t>15.22.1 Scheduling tutors</t>
+  </si>
+  <si>
+    <t>14.13 Lowest common ancestor (LCA)</t>
+  </si>
+  <si>
+    <t>9.11 Lowest common ancestor (LCA)</t>
+  </si>
+  <si>
+    <t>9.12 Lowest common ancestor with parent pointer (LCAP)</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1017,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1031,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1071,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1143,7 +1143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,35 +1342,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
       <c r="I1" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="27" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="16" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1383,10 +1383,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1394,10 +1394,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1405,10 +1405,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1425,10 +1425,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1436,10 +1436,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,10 +1447,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,10 +1458,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1487,10 +1487,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,10 +1533,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1606,12 +1606,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,8 +1657,8 @@
         <v>32</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>243</v>
+      <c r="D34" s="14" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="18" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,7 +1887,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,11 +1940,11 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>19</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,131 +2083,131 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>83</v>
+        <v>263</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="18"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>84</v>
+        <v>264</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="23"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>21</v>
@@ -2216,44 +2216,44 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>19</v>
@@ -2262,16 +2262,16 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>19</v>
@@ -2280,32 +2280,32 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>19</v>
@@ -2314,37 +2314,37 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>19</v>
@@ -2353,23 +2353,23 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>21</v>
@@ -2378,14 +2378,14 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>19</v>
@@ -2394,37 +2394,37 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>21</v>
@@ -2433,16 +2433,16 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>21</v>
@@ -2451,34 +2451,34 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>19</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>19</v>
@@ -2496,23 +2496,23 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>19</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>19</v>
@@ -2530,89 +2530,89 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>19</v>
@@ -2621,50 +2621,50 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>21</v>
@@ -2673,33 +2673,33 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>19</v>
@@ -2708,43 +2708,43 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>19</v>
@@ -2753,7 +2753,7 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>21</v>
@@ -2771,66 +2771,66 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>162</v>
+        <v>262</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>19</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>19</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2857,47 +2857,47 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>21</v>
@@ -2906,18 +2906,18 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
@@ -2926,67 +2926,67 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E189" s="20"/>
       <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C190" s="3"/>
       <c r="D190" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E190" s="25"/>
       <c r="F190" s="21"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>19</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>21</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
@@ -3022,87 +3022,87 @@
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>21</v>
@@ -3111,12 +3111,12 @@
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>19</v>
@@ -3125,25 +3125,25 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C209" s="3"/>
       <c r="D209" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C210" s="3"/>
       <c r="D210" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>21</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>21</v>
@@ -3161,45 +3161,45 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C214" s="3"/>
       <c r="D214" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C216" s="3"/>
       <c r="D216" s="3"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>19</v>
@@ -3208,26 +3208,26 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C220" s="3"/>
       <c r="D220" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>19</v>
@@ -3236,16 +3236,16 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>21</v>
@@ -3254,75 +3254,75 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C225" s="3"/>
       <c r="D225" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B226" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C227" s="3"/>
       <c r="D227" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C230" s="3"/>
       <c r="D230" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>19</v>
@@ -3331,84 +3331,84 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C239" s="3"/>
       <c r="D239" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>21</v>
@@ -3417,59 +3417,59 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>19</v>
@@ -3508,22 +3508,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPI 6.9, big integer multiplication
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -1017,8 +1017,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1031,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1071,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1143,7 +1143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1605,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="14" t="s">
         <v>239</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating CV, part 2
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="E220" sqref="E220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,7 +1616,7 @@
       <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">

</xml_diff>

<commit_message>
EPI 7.0, adding two integers given as lists
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="266">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>9.12 Lowest common ancestor with parent pointer (LCAP)</t>
+  </si>
+  <si>
+    <t>7.0 Add two integers</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1020,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1034,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1074,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1143,7 +1146,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1317,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L249"/>
+  <dimension ref="A1:L250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="E220" sqref="E220"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,16 +1746,16 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>44</v>
+        <v>265</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
@@ -1761,34 +1764,34 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
@@ -1797,54 +1800,52 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C52" s="3"/>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="14" t="s">
-        <v>239</v>
+      <c r="D53" s="18" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
-        <v>241</v>
+      <c r="D54" s="14" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>19</v>
@@ -1854,640 +1855,642 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="B57" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="9" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="9" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>67</v>
+        <v>253</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>239</v>
+      <c r="D69" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D72" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73" s="3" t="s">
+      <c r="C74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="3"/>
-      <c r="D76" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C79" s="3"/>
-      <c r="D79" s="14" t="s">
-        <v>238</v>
-      </c>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80" s="3"/>
-      <c r="D80" s="3" t="s">
-        <v>240</v>
+      <c r="D80" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D84" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C86" s="3"/>
-      <c r="D86" s="18" t="s">
-        <v>238</v>
-      </c>
+      <c r="D86" s="18"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>83</v>
+        <v>264</v>
       </c>
       <c r="C87" s="3"/>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="18" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" s="3" t="s">
+      <c r="C89" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>242</v>
+        <v>88</v>
       </c>
       <c r="C93" s="3"/>
-      <c r="D93" s="23"/>
+      <c r="D93" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>89</v>
+        <v>242</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="D94" s="23"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="18" t="s">
-        <v>238</v>
+        <v>91</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>241</v>
+        <v>92</v>
+      </c>
+      <c r="C98" s="3"/>
+      <c r="D98" s="18" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="9" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="3" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3" t="s">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="12" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="C104" s="3"/>
-      <c r="D104" s="3" t="s">
+      <c r="D104" s="18" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D105" s="3"/>
+        <v>229</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D107" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3" t="s">
-        <v>241</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="D109" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="14" t="s">
-        <v>239</v>
-      </c>
+      <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="14" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="9" t="s">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="9" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D116" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C119" s="3"/>
       <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C120" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="7" t="s">
+      <c r="C122" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="7" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C126" s="3"/>
       <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3" t="s">
+      <c r="C128" s="3"/>
+      <c r="D128" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="12" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C129" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D128" s="3"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C129" s="3"/>
-      <c r="D129" s="14" t="s">
-        <v>238</v>
-      </c>
+      <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C130" s="3"/>
-      <c r="D130" s="3" t="s">
-        <v>239</v>
+      <c r="D130" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C131" s="3"/>
-      <c r="D131" s="18" t="s">
-        <v>238</v>
+      <c r="D131" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D132" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="18" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>19</v>
@@ -2496,32 +2499,32 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C134" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C135" s="3"/>
-      <c r="D135" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D136" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>19</v>
@@ -2530,230 +2533,230 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3" t="s">
+      <c r="C139" s="3"/>
+      <c r="D139" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="7" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C140" s="3"/>
-      <c r="D140" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
+      <c r="D142" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C144" s="3"/>
-      <c r="D144" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D144" s="3"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D148" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
+      <c r="D150" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C151" s="3"/>
-      <c r="D151" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
+      <c r="D152" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D153" s="17" t="s">
-        <v>241</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D154" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C154" s="3" t="s">
+      <c r="C155" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D154" s="3"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="7" t="s">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="11" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="11" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
+      <c r="D158" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C159" s="3"/>
       <c r="D159" s="3"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C160" s="3"/>
-      <c r="D160" s="18" t="s">
-        <v>239</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D160" s="3"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C161" s="3"/>
-      <c r="D161" s="14" t="s">
-        <v>238</v>
+      <c r="D161" s="18" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C162" s="3"/>
-      <c r="D162" s="3" t="s">
-        <v>241</v>
+      <c r="D162" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D164" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -2762,84 +2765,84 @@
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D166" s="3"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D167" s="3"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>245</v>
+        <v>159</v>
       </c>
       <c r="C168" s="3"/>
-      <c r="D168" s="14" t="s">
-        <v>238</v>
+      <c r="D168" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C169" s="3"/>
-      <c r="D169" s="18" t="s">
-        <v>241</v>
+      <c r="D169" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
+      <c r="D170" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C172" s="3"/>
-      <c r="D172" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D172" s="3"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D174" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>19</v>
@@ -2848,110 +2851,108 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C176" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D176" s="3"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B177" s="11" t="s">
+      <c r="C177" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B178" s="11" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B178" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C178" s="3"/>
-      <c r="D178" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B181" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="7" t="s">
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B182" s="9" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B183" s="9" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B183" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D183" s="3"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D185" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B187" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B187" s="9" t="s">
+      <c r="C187" s="3"/>
+      <c r="D187" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B188" s="9" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B188" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D188" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>235</v>
@@ -2959,61 +2960,63 @@
       <c r="D189" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="E189" s="20"/>
-      <c r="F189" s="21"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C190" s="3"/>
+        <v>249</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>235</v>
+      </c>
       <c r="D190" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E190" s="25"/>
+        <v>238</v>
+      </c>
+      <c r="E190" s="20"/>
       <c r="F190" s="21"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>238</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="C191" s="3"/>
+      <c r="D191" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E191" s="25"/>
+      <c r="F191" s="21"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D192" s="14"/>
+        <v>235</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D193" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="D193" s="14"/>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D194" s="3"/>
+      <c r="D194" s="19"/>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
@@ -3022,119 +3025,119 @@
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D196" s="3"/>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="C197" s="3"/>
-      <c r="D197" s="17" t="s">
-        <v>238</v>
+      <c r="D197" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="14" t="s">
-        <v>239</v>
+      <c r="D198" s="17" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
+      <c r="D199" s="14" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C200" s="3"/>
-      <c r="D200" s="3" t="s">
-        <v>241</v>
-      </c>
+      <c r="D200" s="3"/>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C202" s="3"/>
-      <c r="D202" s="3"/>
+      <c r="D202" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C206" s="3" t="s">
+      <c r="C207" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D206" s="3"/>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="9" t="s">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208" s="9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C209" s="3"/>
-      <c r="D209" s="14" t="s">
-        <v>238</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D209" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C210" s="3"/>
       <c r="D210" s="14" t="s">
@@ -3143,16 +3146,16 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D211" s="3"/>
+        <v>260</v>
+      </c>
+      <c r="C211" s="3"/>
+      <c r="D211" s="14" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>21</v>
@@ -3161,209 +3164,209 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D213" s="3" t="s">
-        <v>241</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D213" s="3"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="14" t="s">
-        <v>239</v>
+        <v>194</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D215" s="3" t="s">
-        <v>241</v>
+        <v>195</v>
+      </c>
+      <c r="C215" s="3"/>
+      <c r="D215" s="14" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C217" s="3"/>
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C217" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D217" s="3"/>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="7" t="s">
+      <c r="C218" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="9" t="s">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B220" s="9" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D221" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D223" s="3"/>
+        <v>202</v>
+      </c>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C224" s="3"/>
-      <c r="D224" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D224" s="3"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C225" s="3"/>
       <c r="D225" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B226" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C226" s="3"/>
+      <c r="D226" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="9" t="s">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B227" s="9" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B227" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C227" s="3"/>
-      <c r="D227" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C228" s="3"/>
-      <c r="D228" s="3"/>
+      <c r="D228" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C229" s="3"/>
-      <c r="D229" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D229" s="3"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C230" s="3"/>
       <c r="D230" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C231" s="3"/>
       <c r="D231" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D232" s="3"/>
+      <c r="D232" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B234" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3" t="s">
+      <c r="C234" s="3"/>
+      <c r="D234" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="7" t="s">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="7" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B235" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C235" s="3"/>
-      <c r="D235" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
       <c r="C236" s="3"/>
-      <c r="D236" s="14" t="s">
-        <v>238</v>
+      <c r="D236" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="14" t="s">
@@ -3372,109 +3375,118 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C238" s="3"/>
-      <c r="D238" s="24" t="s">
-        <v>239</v>
+      <c r="D238" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="C239" s="3"/>
-      <c r="D239" s="3" t="s">
-        <v>241</v>
+      <c r="D239" s="24" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="C240" s="3"/>
       <c r="D240" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C241" s="3"/>
-      <c r="D241" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="C242" s="3"/>
       <c r="D242" s="3"/>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C243" s="3"/>
+        <v>221</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D243" s="3"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C244" s="3"/>
-      <c r="D244" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D244" s="3"/>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C249" s="3"/>
+      <c r="D249" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C249" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D249" s="3"/>
+      <c r="C250" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D250" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
EPI 16.1, searching a maze, part 1
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1322,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
       <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
@@ -3233,7 +3233,7 @@
         <v>200</v>
       </c>
       <c r="C221" s="3"/>
-      <c r="D221" s="3" t="s">
+      <c r="D221" s="19" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 13.14, 3-sum: check, all, unique
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="267">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -312,9 +312,6 @@
     <t>11.2 Search a sorted array for the first element larger than k</t>
   </si>
   <si>
-    <t>11.4 Search for a pair in abs-sorted array</t>
-  </si>
-  <si>
     <t>11.5 Search a cyclically sorted array</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
   </si>
   <si>
     <t>13.2 Variable length sort</t>
-  </si>
-  <si>
-    <t>13.3. Least distance sorting</t>
   </si>
   <si>
     <t>13.4 Counting sort</t>
@@ -837,6 +831,15 @@
   </si>
   <si>
     <t>7.0 Add two integers</t>
+  </si>
+  <si>
+    <t>11.4.1 Search for a pair in abs-sorted array</t>
+  </si>
+  <si>
+    <t>11.4.2 Search for a pair in an array (2-sum)</t>
+  </si>
+  <si>
+    <t>13.3 Least distance sorting</t>
   </si>
 </sst>
 </file>
@@ -1320,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L250"/>
+  <dimension ref="A1:L251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,35 +1348,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
       <c r="I1" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1386,10 +1389,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1397,10 +1400,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1408,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1420,7 +1423,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1428,10 +1431,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1439,10 +1442,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1450,10 +1453,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,10 +1464,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1472,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1490,10 +1493,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1509,7 +1512,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,10 +1539,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,7 +1560,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1578,7 +1581,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1609,12 +1612,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1634,7 +1637,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1652,7 +1655,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1661,7 +1664,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,7 +1680,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1691,7 +1694,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1700,7 +1703,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1716,7 +1719,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1725,7 +1728,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,7 +1739,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,11 +1749,11 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,7 +1762,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1768,7 +1771,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,7 +1780,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,7 +1789,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,7 +1798,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,7 +1807,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,7 +1816,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,7 +1825,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,7 +1834,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +1843,7 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,7 +1854,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1862,7 +1865,7 @@
         <v>19</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,7 +1884,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1893,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,7 +1902,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1908,7 +1911,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,7 +1920,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +1929,7 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,7 +1945,7 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,11 +1955,11 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1965,7 +1968,7 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,7 +1984,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2001,7 +2004,7 @@
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +2025,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,7 +2048,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2054,7 +2057,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,7 +2066,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,7 +2075,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2081,7 +2084,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,18 +2098,18 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,7 +2118,7 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,7 +2129,7 @@
         <v>19</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,7 +2143,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,7 +2152,7 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,12 +2161,12 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="23"/>
@@ -2174,7 +2177,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2186,7 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2194,7 +2197,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,7 +2206,7 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,7 +2217,7 @@
         <v>19</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,7 +2236,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,8 +2244,8 @@
         <v>96</v>
       </c>
       <c r="C103" s="3"/>
-      <c r="D103" s="3" t="s">
-        <v>239</v>
+      <c r="D103" s="18" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2251,21 +2254,21 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C105" s="3"/>
-      <c r="D105" s="3" t="s">
-        <v>238</v>
+      <c r="D105" s="18" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>98</v>
+        <v>264</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>19</v>
@@ -2274,232 +2277,232 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>99</v>
+        <v>265</v>
       </c>
       <c r="C107" s="3"/>
-      <c r="D107" s="3" t="s">
-        <v>240</v>
+      <c r="D107" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D108" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3" t="s">
-        <v>241</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="14" t="s">
-        <v>239</v>
-      </c>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D112" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="C112" s="3"/>
+      <c r="D112" s="14" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C113" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="9" t="s">
-        <v>107</v>
-      </c>
+      <c r="B114" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3" t="s">
-        <v>241</v>
+      <c r="B115" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D117" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C121" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="D126" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="C130" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D129" s="3"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C130" s="3"/>
-      <c r="D130" s="14" t="s">
-        <v>238</v>
-      </c>
+      <c r="D130" s="3"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C131" s="3"/>
-      <c r="D131" s="3" t="s">
-        <v>239</v>
+      <c r="D131" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C132" s="3"/>
-      <c r="D132" s="18" t="s">
-        <v>238</v>
+      <c r="D132" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D133" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="18" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>19</v>
@@ -2508,32 +2511,32 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C135" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C136" s="3"/>
-      <c r="D136" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C137" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>19</v>
@@ -2542,212 +2545,212 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
+      <c r="D143" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>137</v>
+        <v>266</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C145" s="3"/>
-      <c r="D145" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D145" s="3"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>208</v>
+        <v>136</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D149" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C150" s="3"/>
-      <c r="D150" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
+      <c r="D151" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C152" s="3"/>
-      <c r="D152" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D154" s="17" t="s">
-        <v>241</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C155" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D155" s="3"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="D156" s="3"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="11" t="s">
-        <v>171</v>
+      <c r="A157" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3" t="s">
-        <v>238</v>
+      <c r="B158" s="11" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
+      <c r="D159" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C160" s="3"/>
       <c r="D160" s="3"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C161" s="3"/>
-      <c r="D161" s="18" t="s">
-        <v>239</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D161" s="3"/>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C162" s="3"/>
-      <c r="D162" s="14" t="s">
-        <v>238</v>
+      <c r="D162" s="18" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C163" s="3"/>
-      <c r="D163" s="3" t="s">
-        <v>241</v>
+      <c r="D163" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3" t="s">
@@ -2756,16 +2759,16 @@
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D165" s="3"/>
+        <v>153</v>
+      </c>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>19</v>
@@ -2774,84 +2777,84 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D167" s="3"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D168" s="3"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="C169" s="3"/>
-      <c r="D169" s="14" t="s">
+      <c r="D169" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="C170" s="3"/>
-      <c r="D170" s="18" t="s">
-        <v>241</v>
+      <c r="D170" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>160</v>
+        <v>260</v>
       </c>
       <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
+      <c r="D171" s="18" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C173" s="3"/>
-      <c r="D173" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D173" s="3"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D175" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2860,7 +2863,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>19</v>
@@ -2868,164 +2871,164 @@
       <c r="D177" s="3"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B178" s="11" t="s">
-        <v>167</v>
-      </c>
+      <c r="B178" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D178" s="3"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B179" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3" t="s">
-        <v>241</v>
+      <c r="B179" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B181" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B182" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B183" s="9" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B184" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D184" s="3"/>
+      <c r="B184" s="9" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D185" s="3"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D186" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B188" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B189" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B188" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B189" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D189" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E190" s="20"/>
-      <c r="F190" s="21"/>
+        <v>236</v>
+      </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C191" s="3"/>
+        <v>247</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="D191" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E191" s="25"/>
+        <v>236</v>
+      </c>
+      <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>238</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="C192" s="3"/>
+      <c r="D192" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E192" s="25"/>
+      <c r="F192" s="21"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D193" s="14"/>
+        <v>233</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D194" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="D194" s="14"/>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>179</v>
+        <v>249</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D195" s="3"/>
+      <c r="D195" s="19"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>21</v>
@@ -3034,137 +3037,137 @@
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D197" s="3"/>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>258</v>
+        <v>179</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="17" t="s">
+      <c r="D198" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="14" t="s">
-        <v>239</v>
+      <c r="D199" s="17" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="C200" s="3"/>
-      <c r="D200" s="3"/>
+      <c r="D200" s="14" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="D201" s="3" t="s">
-        <v>241</v>
-      </c>
+      <c r="D201" s="3"/>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C203" s="3"/>
-      <c r="D203" s="3"/>
+      <c r="D203" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B209" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C207" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D207" s="3"/>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B209" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D209" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C210" s="3"/>
-      <c r="D210" s="14" t="s">
-        <v>238</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D210" s="3"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D212" s="3"/>
+        <v>258</v>
+      </c>
+      <c r="C212" s="3"/>
+      <c r="D212" s="14" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>21</v>
@@ -3173,148 +3176,148 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D214" s="3" t="s">
-        <v>241</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C215" s="3"/>
-      <c r="D215" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D215" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>241</v>
+        <v>193</v>
+      </c>
+      <c r="C216" s="3"/>
+      <c r="D216" s="14" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
+        <v>194</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="7" t="s">
-        <v>199</v>
-      </c>
+      <c r="B219" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D219" s="3"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="9" t="s">
-        <v>206</v>
+      <c r="A220" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B221" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C221" s="3"/>
-      <c r="D221" s="19" t="s">
-        <v>238</v>
+      <c r="B221" s="9" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D222" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="C222" s="3"/>
+      <c r="D222" s="14" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D224" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C225" s="3"/>
-      <c r="D225" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D225" s="3"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B227" s="9" t="s">
-        <v>207</v>
+      <c r="B227" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C227" s="3"/>
+      <c r="D227" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B228" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C228" s="3"/>
-      <c r="D228" s="3" t="s">
-        <v>238</v>
+      <c r="B228" s="9" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C229" s="3"/>
-      <c r="D229" s="3"/>
+      <c r="D229" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C230" s="3"/>
-      <c r="D230" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="D230" s="3"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3" t="s">
@@ -3323,170 +3326,179 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="C232" s="3"/>
       <c r="D232" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D233" s="3"/>
+      <c r="D233" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3" t="s">
-        <v>241</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D234" s="3"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="7" t="s">
-        <v>216</v>
+      <c r="B235" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B236" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C236" s="3"/>
-      <c r="D236" s="3" t="s">
-        <v>240</v>
+      <c r="A236" s="7" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="C237" s="3"/>
-      <c r="D237" s="14" t="s">
+      <c r="D237" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C238" s="3"/>
       <c r="D238" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C239" s="3"/>
-      <c r="D239" s="24" t="s">
-        <v>239</v>
+      <c r="D239" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="C240" s="3"/>
-      <c r="D240" s="3" t="s">
-        <v>241</v>
+      <c r="D240" s="24" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="C241" s="3"/>
       <c r="D241" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C242" s="3"/>
-      <c r="D242" s="3"/>
+        <v>217</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C243" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="C243" s="3"/>
       <c r="D243" s="3"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C244" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D244" s="3"/>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C245" s="3"/>
-      <c r="D245" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D245" s="3"/>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D250" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="C250" s="3"/>
+      <c r="D250" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B251" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D251" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3520,22 +3532,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPI 7.1, merging sorted SL-lists
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Personal\03_Projects\Interview\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="267">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -845,7 +850,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -888,7 +893,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,12 +935,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -974,7 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1012,7 +1011,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1031,6 +1029,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1079,7 +1080,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1114,7 +1115,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1325,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,11 +1351,11 @@
       <c r="D1" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
         <v>230</v>
       </c>
@@ -1365,11 +1366,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
         <v>231</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="14" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2169,7 +2170,9 @@
         <v>240</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="23"/>
+      <c r="D94" s="14" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
@@ -2994,7 +2997,7 @@
       <c r="D192" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="E192" s="25"/>
+      <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
@@ -3399,7 +3402,7 @@
         <v>254</v>
       </c>
       <c r="C240" s="3"/>
-      <c r="D240" s="24" t="s">
+      <c r="D240" s="23" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 16.10.1. Shortest Path (Dijkstra Algorithm), min-heap implementation
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="268">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -651,9 +651,6 @@
   </si>
   <si>
     <t>16.9 Shortest path with fewest edges</t>
-  </si>
-  <si>
-    <t>16.10 Quickest route</t>
   </si>
   <si>
     <t>16.11 Road network</t>
@@ -845,6 +842,12 @@
   </si>
   <si>
     <t>13.3 Least distance sorting</t>
+  </si>
+  <si>
+    <t>16.10.1 Sortest Path (Dijkstra Algorithm)</t>
+  </si>
+  <si>
+    <t>16.10.2 Quickest route</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L251"/>
+  <dimension ref="A1:L252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,35 +1352,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1390,10 +1393,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1401,10 +1404,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1412,10 +1415,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1424,7 +1427,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1432,10 +1435,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1443,10 +1446,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1454,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1465,10 +1468,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1476,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1494,10 +1497,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1513,7 +1516,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,10 +1543,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1561,7 +1564,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,7 +1585,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1613,12 +1616,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1638,7 +1641,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1656,7 +1659,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1665,7 +1668,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,7 +1684,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,7 +1698,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,7 +1707,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,7 +1723,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,7 +1732,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1740,7 +1743,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1750,11 +1753,11 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1763,7 +1766,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1772,7 +1775,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,7 +1784,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,7 +1793,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,7 +1802,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,7 +1811,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1820,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,7 +1829,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1838,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1844,7 +1847,7 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,7 +1858,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1869,7 @@
         <v>19</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,7 +1888,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1894,7 +1897,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,7 +1906,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,7 +1915,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,7 +1924,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,7 +1933,7 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,7 +1949,7 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,11 +1959,11 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +1972,7 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1988,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2005,7 +2008,7 @@
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,7 +2029,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,7 +2052,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2061,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,7 +2070,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2076,7 +2079,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2085,7 +2088,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,18 +2102,18 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,7 +2122,7 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,7 +2133,7 @@
         <v>19</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,7 +2147,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2156,7 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,16 +2165,16 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2180,7 +2183,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,7 +2192,7 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,7 +2203,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,7 +2212,7 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2220,7 +2223,7 @@
         <v>19</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2248,7 +2251,7 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,21 +2260,21 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>19</v>
@@ -2280,11 +2283,11 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2293,7 +2296,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2311,7 +2314,7 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,7 +2330,7 @@
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,7 +2360,7 @@
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,7 +2369,7 @@
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2384,7 +2387,7 @@
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2430,7 +2433,7 @@
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2439,7 +2442,7 @@
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,7 +2467,7 @@
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,7 +2485,7 @@
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2491,7 +2494,7 @@
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,8 +2502,8 @@
         <v>124</v>
       </c>
       <c r="C133" s="3"/>
-      <c r="D133" s="18" t="s">
-        <v>236</v>
+      <c r="D133" s="19" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,7 +2537,7 @@
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2561,7 +2564,7 @@
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2575,7 +2578,7 @@
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2584,12 +2587,12 @@
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -2607,7 +2610,7 @@
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2616,7 +2619,7 @@
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2625,7 +2628,7 @@
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,7 +2637,7 @@
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,8 +2654,8 @@
         <v>140</v>
       </c>
       <c r="C151" s="3"/>
-      <c r="D151" s="3" t="s">
-        <v>237</v>
+      <c r="D151" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2668,7 +2671,7 @@
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,7 +2689,7 @@
         <v>19</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,7 +2717,7 @@
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2739,7 +2742,7 @@
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
@@ -2748,7 +2751,7 @@
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
@@ -2757,7 +2760,7 @@
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
@@ -2766,7 +2769,7 @@
       </c>
       <c r="C165" s="3"/>
       <c r="D165" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
@@ -2802,25 +2805,25 @@
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
@@ -2843,7 +2846,7 @@
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
@@ -2852,7 +2855,7 @@
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
@@ -2893,7 +2896,7 @@
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -2902,7 +2905,7 @@
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -2939,7 +2942,7 @@
         <v>19</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -2957,7 +2960,7 @@
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -2967,53 +2970,53 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>19</v>
@@ -3022,7 +3025,7 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
@@ -3053,25 +3056,25 @@
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
@@ -3087,7 +3090,7 @@
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
@@ -3096,7 +3099,7 @@
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
@@ -3152,20 +3155,20 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,7 +3197,7 @@
         <v>19</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -3203,7 +3206,7 @@
       </c>
       <c r="C216" s="3"/>
       <c r="D216" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3214,7 +3217,7 @@
         <v>19</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3249,7 +3252,7 @@
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3267,7 +3270,7 @@
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,7 +3288,7 @@
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -3294,7 +3297,7 @@
       </c>
       <c r="C227" s="3"/>
       <c r="D227" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,7 +3311,7 @@
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,152 +3327,152 @@
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="C232" s="3"/>
-      <c r="D232" s="3" t="s">
-        <v>236</v>
+      <c r="D232" s="14" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="C233" s="3"/>
       <c r="D233" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D234" s="3"/>
+      <c r="D234" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B236" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="C235" s="3"/>
-      <c r="D235" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B237" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C237" s="3"/>
-      <c r="D237" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="C238" s="3"/>
-      <c r="D238" s="14" t="s">
-        <v>236</v>
+      <c r="D238" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C239" s="3"/>
       <c r="D239" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C240" s="3"/>
-      <c r="D240" s="23" t="s">
-        <v>237</v>
+      <c r="D240" s="14" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>216</v>
+        <v>253</v>
       </c>
       <c r="C241" s="3"/>
-      <c r="D241" s="3" t="s">
-        <v>239</v>
+      <c r="D241" s="23" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C243" s="3"/>
-      <c r="D243" s="3"/>
+        <v>216</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C244" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="C244" s="3"/>
       <c r="D244" s="3"/>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C245" s="3"/>
+        <v>218</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D245" s="3"/>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C246" s="3"/>
-      <c r="D246" s="3" t="s">
-        <v>236</v>
-      </c>
+      <c r="D246" s="3"/>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3" t="s">
@@ -3478,30 +3481,39 @@
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D251" s="3"/>
+        <v>224</v>
+      </c>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D252" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3535,22 +3547,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPI 16.10.4, Minimum Spannin Tree - MST (Prim's Algorithm)
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="272">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>16.9 Shortest path with fewest edges</t>
+  </si>
+  <si>
+    <t>16.10 Quickest route</t>
   </si>
   <si>
     <t>16.11 Road network</t>
@@ -844,10 +847,19 @@
     <t>13.3 Least distance sorting</t>
   </si>
   <si>
-    <t>16.10.1 Sortest Path (Dijkstra Algorithm)</t>
-  </si>
-  <si>
-    <t>16.10.2 Quickest route</t>
+    <t>16.0.1 Breadth-first search (BFS)</t>
+  </si>
+  <si>
+    <t>16.0.2 Depth-first search (DFS)</t>
+  </si>
+  <si>
+    <t>16.0.3 Shortest Path (Dijkstra)</t>
+  </si>
+  <si>
+    <t>16.0.4 Minimum spanning tree (MST, Prim's)</t>
+  </si>
+  <si>
+    <t>16.0.5 Minimum spanning tree (MST, Kruskal's)</t>
   </si>
 </sst>
 </file>
@@ -1327,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L252"/>
+  <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="D233" sqref="D233"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,35 +1364,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1393,10 +1405,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1404,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1415,10 +1427,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1427,7 +1439,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1435,10 +1447,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1446,10 +1458,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1457,10 +1469,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1468,10 +1480,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1479,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1497,10 +1509,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1516,7 +1528,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,10 +1555,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1576,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1597,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1616,12 +1628,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1641,7 +1653,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,7 +1671,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,7 +1680,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1684,7 +1696,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1698,7 +1710,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1707,7 +1719,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1735,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,7 +1744,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1743,7 +1755,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,11 +1765,11 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,7 +1778,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,7 +1787,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1796,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,7 +1805,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1802,7 +1814,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1811,7 +1823,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,7 +1832,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1841,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="18" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1838,7 +1850,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,7 +1859,7 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,7 +1870,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,7 +1881,7 @@
         <v>19</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1900,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,7 +1909,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,7 +1918,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,7 +1927,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,7 +1936,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,7 +1945,7 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1961,7 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1959,11 +1971,11 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,7 +1984,7 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,7 +2000,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,7 +2041,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2052,7 +2064,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,7 +2073,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,7 +2082,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,7 +2091,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,7 +2100,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,18 +2114,18 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="18"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2122,7 +2134,7 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2133,7 +2145,7 @@
         <v>19</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,7 +2159,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2156,7 +2168,7 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,16 +2177,16 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2195,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2192,7 +2204,7 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,7 +2215,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,7 +2224,7 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2223,7 +2235,7 @@
         <v>19</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2251,7 +2263,7 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,21 +2272,21 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="18" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>19</v>
@@ -2283,11 +2295,11 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,7 +2308,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,7 +2326,7 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2330,7 +2342,7 @@
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2360,7 +2372,7 @@
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,7 +2381,7 @@
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2387,7 +2399,7 @@
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2433,7 +2445,7 @@
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2442,7 +2454,7 @@
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2467,7 +2479,7 @@
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,7 +2497,7 @@
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,7 +2506,7 @@
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,7 +2515,7 @@
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,7 +2549,7 @@
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,7 +2576,7 @@
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,7 +2590,7 @@
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2587,12 +2599,12 @@
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -2610,7 +2622,7 @@
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,7 +2631,7 @@
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2628,7 +2640,7 @@
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,7 +2649,7 @@
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2655,7 +2667,7 @@
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,7 +2683,7 @@
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2689,7 +2701,7 @@
         <v>19</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,7 +2729,7 @@
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2742,7 +2754,7 @@
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="18" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
@@ -2751,7 +2763,7 @@
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
@@ -2760,7 +2772,7 @@
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
@@ -2769,7 +2781,7 @@
       </c>
       <c r="C165" s="3"/>
       <c r="D165" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
@@ -2805,25 +2817,25 @@
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="18" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
@@ -2846,7 +2858,7 @@
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
@@ -2855,7 +2867,7 @@
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
@@ -2896,7 +2908,7 @@
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -2905,7 +2917,7 @@
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -2942,7 +2954,7 @@
         <v>19</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -2960,7 +2972,7 @@
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -2970,53 +2982,53 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>19</v>
@@ -3025,7 +3037,7 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
@@ -3056,25 +3068,25 @@
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
@@ -3090,7 +3102,7 @@
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
@@ -3099,7 +3111,7 @@
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
@@ -3155,20 +3167,20 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,7 +3209,7 @@
         <v>19</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -3206,7 +3218,7 @@
       </c>
       <c r="C216" s="3"/>
       <c r="D216" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3217,7 +3229,7 @@
         <v>19</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3248,177 +3260,177 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>198</v>
+        <v>267</v>
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D223" s="3"/>
+        <v>268</v>
+      </c>
+      <c r="C223" s="3"/>
+      <c r="D223" s="14" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C224" s="3"/>
+      <c r="D224" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B225" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B226" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C224" s="3"/>
-      <c r="D224" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D225" s="3"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B228" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C228" s="3"/>
+      <c r="D228" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B229" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C227" s="3"/>
-      <c r="D227" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B228" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B229" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B230" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C230" s="3"/>
-      <c r="D230" s="3"/>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B230" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="C231" s="3"/>
-      <c r="D231" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C233" s="3"/>
-      <c r="D233" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D233" s="18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="7" t="s">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B238" s="3" t="s">
+      <c r="C240" s="3"/>
+      <c r="D240" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C238" s="3"/>
-      <c r="D238" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B239" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C239" s="3"/>
-      <c r="D239" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B240" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C240" s="3"/>
-      <c r="D240" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B241" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C241" s="3"/>
-      <c r="D241" s="23" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
         <v>215</v>
       </c>
@@ -3427,93 +3439,129 @@
         <v>238</v>
       </c>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C243" s="3"/>
+      <c r="D243" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B244" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C244" s="3"/>
+      <c r="D244" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B245" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C245" s="3"/>
+      <c r="D245" s="23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B246" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="3" t="s">
+      <c r="C246" s="3"/>
+      <c r="D246" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B247" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C244" s="3"/>
-      <c r="D244" s="3"/>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B245" s="3" t="s">
+      <c r="C247" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C245" s="3" t="s">
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B249" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C249" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D245" s="3"/>
-    </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B246" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C246" s="3"/>
-      <c r="D246" s="3"/>
-    </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B247" s="3" t="s">
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C247" s="3"/>
-      <c r="D247" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B248" s="3" t="s">
+      <c r="C250" s="3"/>
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B251" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C248" s="3"/>
-      <c r="D248" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B249" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C249" s="3"/>
-      <c r="D249" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C250" s="3"/>
-      <c r="D250" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B251" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B252" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C252" s="3"/>
+      <c r="D252" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B253" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C253" s="3"/>
+      <c r="D253" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B254" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C254" s="3"/>
+      <c r="D254" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B255" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D252" s="3"/>
+      <c r="C255" s="3"/>
+      <c r="D255" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B256" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D256" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3547,22 +3595,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructuring in 'Tree Problems'. Adding min/max paths in non-BST tree.
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="272">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="E237" sqref="E237"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2117,9 @@
         <v>261</v>
       </c>
       <c r="C86" s="3"/>
-      <c r="D86" s="18"/>
+      <c r="D86" s="19" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
@@ -2728,7 +2730,7 @@
         <v>147</v>
       </c>
       <c r="C159" s="3"/>
-      <c r="D159" s="3" t="s">
+      <c r="D159" s="14" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2834,7 +2836,7 @@
         <v>260</v>
       </c>
       <c r="C171" s="3"/>
-      <c r="D171" s="18" t="s">
+      <c r="D171" s="14" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2971,7 +2973,7 @@
         <v>174</v>
       </c>
       <c r="C188" s="3"/>
-      <c r="D188" s="3" t="s">
+      <c r="D188" s="18" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding EPI 11.17, Leetcode 136, Unique Number
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2373,7 @@
         <v>107</v>
       </c>
       <c r="C116" s="3"/>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="14" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       <c r="C121" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D121" s="3"/>
+      <c r="D121" s="14"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">

</xml_diff>

<commit_message>
Pramp, all k-diff pairs in an array
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Leetcode 230, K-th Smallest Element in BST
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,7 +1917,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="14" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3294,7 +3294,7 @@
       <c r="C225" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D225" s="3"/>
+      <c r="D225" s="18"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">

</xml_diff>

<commit_message>
EPI 13.8/Leetcode 26, removing duplicates in a sorted array
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -431,9 +431,6 @@
     <t>13.4 Counting sort</t>
   </si>
   <si>
-    <t>13.5 Intersect two sorted arrays</t>
-  </si>
-  <si>
     <t>13.7 Count the occurences of characters in a sentence</t>
   </si>
   <si>
@@ -860,6 +857,9 @@
   </si>
   <si>
     <t>16.0.5 Minimum spanning tree (MST, Kruskal's)</t>
+  </si>
+  <si>
+    <t>13.5 Intersection of two sorted arrays</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
       <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
@@ -1364,35 +1364,35 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1405,10 +1405,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1416,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1427,10 +1427,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,10 +1447,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,10 +1458,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1469,10 +1469,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1480,10 +1480,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1509,10 +1509,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,10 +1555,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1628,12 +1628,12 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1755,7 +1755,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
         <v>19</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,11 +1971,11 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,20 +2114,20 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>19</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,16 +2179,16 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
         <v>19</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,21 +2274,21 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>19</v>
@@ -2297,11 +2297,11 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2601,12 +2601,12 @@
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -2620,43 +2620,43 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>136</v>
+        <v>271</v>
       </c>
       <c r="C146" s="3"/>
-      <c r="D146" s="3" t="s">
-        <v>236</v>
+      <c r="D146" s="14" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C147" s="3"/>
-      <c r="D147" s="3" t="s">
-        <v>237</v>
+      <c r="D147" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C148" s="3"/>
-      <c r="D148" s="3" t="s">
-        <v>238</v>
+      <c r="D148" s="19" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C149" s="3"/>
-      <c r="D149" s="3" t="s">
-        <v>239</v>
+      <c r="D149" s="14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>19</v>
@@ -2665,50 +2665,50 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>21</v>
@@ -2717,33 +2717,33 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>19</v>
@@ -2752,43 +2752,43 @@
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C165" s="3"/>
       <c r="D165" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>19</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>19</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>21</v>
@@ -2815,66 +2815,66 @@
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>19</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>19</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>19</v>
@@ -2901,47 +2901,47 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B181" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
@@ -2950,18 +2950,18 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>21</v>
@@ -2970,67 +2970,67 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>19</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>21</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>21</v>
@@ -3066,87 +3066,87 @@
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>21</v>
@@ -3155,12 +3155,12 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>19</v>
@@ -3169,25 +3169,25 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>21</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>21</v>
@@ -3205,45 +3205,45 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C216" s="3"/>
       <c r="D216" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>19</v>
@@ -3252,44 +3252,44 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>19</v>
@@ -3298,16 +3298,16 @@
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>21</v>
@@ -3316,102 +3316,102 @@
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>19</v>
@@ -3420,84 +3420,84 @@
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>21</v>
@@ -3506,59 +3506,59 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B252" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B253" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B254" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B255" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B256" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>19</v>
@@ -3597,22 +3597,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPI 9.7/EPI 14.7/Leetcode 108, reconstructing BST from a sorted array
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="E225" sqref="E225"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2081,7 @@
         <v>79</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="14" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2782,7 +2782,7 @@
         <v>152</v>
       </c>
       <c r="C165" s="3"/>
-      <c r="D165" s="3" t="s">
+      <c r="D165" s="14" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPI 10.8/Leetcode 295, online median of a stream
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="24920" windowHeight="11960"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -1341,21 +1341,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" customWidth="1"/>
     <col min="2" max="2" width="74" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F2" s="26" t="s">
         <v>228</v>
       </c>
@@ -1395,12 +1395,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1515,14 +1515,14 @@
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1540,17 +1540,17 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1579,14 +1579,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>249</v>
       </c>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="D25" s="18"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>231</v>
       </c>
@@ -1640,14 +1640,14 @@
       </c>
       <c r="D29" s="17"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
@@ -1683,14 +1683,14 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1699,12 +1699,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1722,14 +1722,14 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
         <v>40</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
@@ -1758,12 +1758,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
         <v>262</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B49" s="3" t="s">
         <v>47</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B51" s="3" t="s">
         <v>49</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B53" s="3" t="s">
         <v>50</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>52</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>53</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B56" s="3" t="s">
         <v>54</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
@@ -1884,17 +1884,17 @@
         <v>238</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B59" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B60" s="3" t="s">
         <v>58</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B61" s="3" t="s">
         <v>59</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>60</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B63" s="3" t="s">
         <v>61</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B64" s="3" t="s">
         <v>62</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B65" s="3" t="s">
         <v>63</v>
       </c>
@@ -1948,14 +1948,14 @@
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B66" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B67" s="3" t="s">
         <v>65</v>
       </c>
@@ -1964,12 +1964,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B68" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B69" s="3" t="s">
         <v>250</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B70" s="3" t="s">
         <v>67</v>
       </c>
@@ -1987,14 +1987,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B71" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B72" s="3" t="s">
         <v>69</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B73" s="3" t="s">
         <v>70</v>
       </c>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B74" s="3" t="s">
         <v>71</v>
       </c>
@@ -2023,19 +2023,19 @@
         <v>237</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B76" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B77" s="3" t="s">
         <v>74</v>
       </c>
@@ -2044,21 +2044,21 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B78" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
         <v>77</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
         <v>78</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>79</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
         <v>80</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
         <v>81</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
         <v>82</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B86" s="3" t="s">
         <v>260</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B87" s="3" t="s">
         <v>261</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
         <v>83</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
         <v>84</v>
       </c>
@@ -2150,12 +2150,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
         <v>86</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
         <v>87</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
         <v>88</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B94" s="3" t="s">
         <v>239</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B95" s="3" t="s">
         <v>89</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B96" s="3" t="s">
         <v>90</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B97" s="3" t="s">
         <v>91</v>
       </c>
@@ -2220,16 +2220,16 @@
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B98" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C98" s="3"/>
-      <c r="D98" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B99" s="3" t="s">
         <v>93</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B100" s="3" t="s">
         <v>94</v>
       </c>
@@ -2249,17 +2249,17 @@
       </c>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B102" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B103" s="3" t="s">
         <v>96</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B104" s="12" t="s">
         <v>97</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B105" s="3" t="s">
         <v>226</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B106" s="3" t="s">
         <v>263</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B107" s="3" t="s">
         <v>264</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B108" s="3" t="s">
         <v>98</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B109" s="3" t="s">
         <v>99</v>
       </c>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B110" s="3" t="s">
         <v>100</v>
       </c>
@@ -2331,14 +2331,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B111" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B112" s="3" t="s">
         <v>102</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B113" s="3" t="s">
         <v>103</v>
       </c>
@@ -2356,19 +2356,19 @@
       </c>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B114" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B115" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B116" s="3" t="s">
         <v>107</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B117" s="3" t="s">
         <v>108</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B118" s="3" t="s">
         <v>109</v>
       </c>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B119" s="3" t="s">
         <v>110</v>
       </c>
@@ -2404,14 +2404,14 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B120" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B121" s="3" t="s">
         <v>112</v>
       </c>
@@ -2420,14 +2420,14 @@
       </c>
       <c r="D121" s="14"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B122" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B123" s="3" t="s">
         <v>114</v>
       </c>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B125" s="3" t="s">
         <v>116</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B126" s="3" t="s">
         <v>117</v>
       </c>
@@ -2459,14 +2459,14 @@
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B127" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B128" s="3" t="s">
         <v>119</v>
       </c>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B129" s="3" t="s">
         <v>120</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B130" s="12" t="s">
         <v>121</v>
       </c>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B131" s="3" t="s">
         <v>122</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B132" s="3" t="s">
         <v>123</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B133" s="3" t="s">
         <v>124</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B134" s="3" t="s">
         <v>125</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B135" s="3" t="s">
         <v>126</v>
       </c>
@@ -2538,14 +2538,14 @@
       </c>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B136" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B137" s="3" t="s">
         <v>129</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B138" s="3" t="s">
         <v>128</v>
       </c>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B139" s="3" t="s">
         <v>130</v>
       </c>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B140" s="3" t="s">
         <v>131</v>
       </c>
@@ -2581,12 +2581,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B142" s="3" t="s">
         <v>133</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B143" s="3" t="s">
         <v>134</v>
       </c>
@@ -2604,21 +2604,21 @@
         <v>235</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B144" s="3" t="s">
         <v>265</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B145" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B146" s="3" t="s">
         <v>271</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B147" s="3" t="s">
         <v>205</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B148" s="3" t="s">
         <v>136</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B149" s="3" t="s">
         <v>137</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B150" s="3" t="s">
         <v>138</v>
       </c>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B151" s="3" t="s">
         <v>139</v>
       </c>
@@ -2672,14 +2672,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B152" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B153" s="3" t="s">
         <v>141</v>
       </c>
@@ -2688,14 +2688,14 @@
         <v>235</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B154" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B155" s="3" t="s">
         <v>143</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B156" s="3" t="s">
         <v>144</v>
       </c>
@@ -2715,17 +2715,17 @@
       </c>
       <c r="D156" s="3"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B158" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B159" s="3" t="s">
         <v>146</v>
       </c>
@@ -2734,14 +2734,14 @@
         <v>235</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B160" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="3" t="s">
         <v>148</v>
       </c>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="D161" s="3"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="3" t="s">
         <v>149</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B163" s="3" t="s">
         <v>150</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B164" s="3" t="s">
         <v>151</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="3" t="s">
         <v>152</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="3" t="s">
         <v>153</v>
       </c>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="3" t="s">
         <v>154</v>
       </c>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="D167" s="3"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="3" t="s">
         <v>155</v>
       </c>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B169" s="3" t="s">
         <v>156</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="3" t="s">
         <v>242</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="3" t="s">
         <v>259</v>
       </c>
@@ -2840,21 +2840,21 @@
         <v>238</v>
       </c>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B172" s="3" t="s">
         <v>157</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B174" s="3" t="s">
         <v>159</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="3" t="s">
         <v>160</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="3" t="s">
         <v>161</v>
       </c>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="D176" s="3"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B177" s="3" t="s">
         <v>162</v>
       </c>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="D177" s="3"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B178" s="3" t="s">
         <v>163</v>
       </c>
@@ -2899,12 +2899,12 @@
       </c>
       <c r="D178" s="3"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B179" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B180" s="3" t="s">
         <v>165</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B181" s="3" t="s">
         <v>166</v>
       </c>
@@ -2922,24 +2922,24 @@
         <v>237</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B182" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B184" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B185" s="3" t="s">
         <v>170</v>
       </c>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="D185" s="3"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B186" s="3" t="s">
         <v>171</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B187" s="3" t="s">
         <v>172</v>
       </c>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D187" s="3"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B188" s="3" t="s">
         <v>173</v>
       </c>
@@ -2977,12 +2977,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B189" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B190" s="3" t="s">
         <v>247</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B191" s="3" t="s">
         <v>246</v>
       </c>
@@ -3006,7 +3006,7 @@
       <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B192" s="3" t="s">
         <v>254</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="3" t="s">
         <v>245</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="3" t="s">
         <v>244</v>
       </c>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="D194" s="14"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="3" t="s">
         <v>248</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="D195" s="19"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="3" t="s">
         <v>176</v>
       </c>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B197" s="3" t="s">
         <v>177</v>
       </c>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="3" t="s">
         <v>178</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="3" t="s">
         <v>255</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="3" t="s">
         <v>243</v>
       </c>
@@ -3091,14 +3091,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="3" t="s">
         <v>180</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B203" s="3" t="s">
         <v>181</v>
       </c>
@@ -3116,35 +3116,35 @@
         <v>237</v>
       </c>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="3" t="s">
         <v>182</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B205" s="3" t="s">
         <v>183</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B208" s="3" t="s">
         <v>185</v>
       </c>
@@ -3153,12 +3153,12 @@
       </c>
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B209" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B210" s="3" t="s">
         <v>188</v>
       </c>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="D210" s="3"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B211" s="3" t="s">
         <v>258</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B212" s="3" t="s">
         <v>257</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B213" s="3" t="s">
         <v>189</v>
       </c>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B214" s="3" t="s">
         <v>190</v>
       </c>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B215" s="3" t="s">
         <v>191</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B216" s="3" t="s">
         <v>192</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B217" s="3" t="s">
         <v>193</v>
       </c>
@@ -3234,14 +3234,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B218" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B219" s="3" t="s">
         <v>195</v>
       </c>
@@ -3250,17 +3250,17 @@
       </c>
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B221" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B222" s="3" t="s">
         <v>266</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B223" s="3" t="s">
         <v>267</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B224" s="3" t="s">
         <v>197</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B225" s="3" t="s">
         <v>198</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="D225" s="18"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B226" s="3" t="s">
         <v>199</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B227" s="3" t="s">
         <v>200</v>
       </c>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B228" s="3" t="s">
         <v>201</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="3" t="s">
         <v>202</v>
       </c>
@@ -3332,12 +3332,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B230" s="9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B231" s="3" t="s">
         <v>268</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B232" s="3" t="s">
         <v>269</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="3" t="s">
         <v>270</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B234" s="3" t="s">
         <v>206</v>
       </c>
@@ -3373,14 +3373,14 @@
         <v>235</v>
       </c>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B235" s="3" t="s">
         <v>207</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B236" s="3" t="s">
         <v>208</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B237" s="3" t="s">
         <v>209</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B238" s="3" t="s">
         <v>210</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B239" s="3" t="s">
         <v>211</v>
       </c>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B240" s="3" t="s">
         <v>212</v>
       </c>
@@ -3427,12 +3427,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B242" s="3" t="s">
         <v>214</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B243" s="3" t="s">
         <v>251</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B244" s="3" t="s">
         <v>252</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B245" s="3" t="s">
         <v>253</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B246" s="3" t="s">
         <v>215</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B247" s="3" t="s">
         <v>216</v>
       </c>
@@ -3488,14 +3488,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B248" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B249" s="3" t="s">
         <v>218</v>
       </c>
@@ -3504,14 +3504,14 @@
       </c>
       <c r="D249" s="3"/>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B250" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B251" s="3" t="s">
         <v>220</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B252" s="3" t="s">
         <v>221</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B253" s="3" t="s">
         <v>222</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B254" s="3" t="s">
         <v>223</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B255" s="3" t="s">
         <v>224</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B256" s="3" t="s">
         <v>225</v>
       </c>
@@ -3593,24 +3593,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>238</v>
       </c>
@@ -3626,7 +3626,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPI 10.5/Leetcode 215/703, k-th largest element of an array/stream
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="24920" windowHeight="11960"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="24915" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="272">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -305,9 +305,6 @@
     <t>10.9 Generating numbers in form a + b*sqrt(q)</t>
   </si>
   <si>
-    <t>10.10 Comparing with the k-th largets element</t>
-  </si>
-  <si>
     <t>11.Searching</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
   </si>
   <si>
     <t>11.12 Finding min and max simultaneously</t>
-  </si>
-  <si>
-    <t>11.13 The k-th largest element</t>
   </si>
   <si>
     <t>11.14 The k-th largest element, large n and small k</t>
@@ -860,6 +854,12 @@
   </si>
   <si>
     <t>13.5 Intersection of two sorted arrays</t>
+  </si>
+  <si>
+    <t>11.13 The k-th largest element at O(n)</t>
+  </si>
+  <si>
+    <t>10.10 Comparing with the k-th largest element</t>
   </si>
 </sst>
 </file>
@@ -1341,21 +1341,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="74" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1364,138 +1364,138 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F2" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
       <c r="I2" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1504,34 +1504,34 @@
       </c>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1540,28 +1540,28 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1570,23 +1570,23 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1595,16 +1595,16 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="18"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1622,41 +1622,43 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D29" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1665,89 +1667,89 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="18" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
@@ -1755,114 +1757,114 @@
         <v>19</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="18" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>54</v>
       </c>
@@ -1870,10 +1872,10 @@
         <v>19</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
@@ -1881,129 +1883,129 @@
         <v>19</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>70</v>
       </c>
@@ -2012,7 +2014,7 @@
       </c>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>71</v>
       </c>
@@ -2020,90 +2022,90 @@
         <v>19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>82</v>
       </c>
@@ -2112,34 +2114,34 @@
       </c>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
         <v>84</v>
       </c>
@@ -2147,69 +2149,69 @@
         <v>19</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B94" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C95" s="3"/>
-      <c r="D95" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D95" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
         <v>91</v>
       </c>
@@ -2217,19 +2219,19 @@
         <v>19</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
         <v>93</v>
       </c>
@@ -2237,1328 +2239,1328 @@
         <v>19</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
-        <v>94</v>
+        <v>271</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B102" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B103" s="3" t="s">
+      <c r="C103" s="3"/>
+      <c r="D103" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B104" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="C104" s="3"/>
-      <c r="D104" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D104" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D109" s="3"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B110" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" s="17"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" s="3"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B114" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="3" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B116" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" s="23"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B118" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D118" s="3"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B119" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D121" s="14"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D123" s="3"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A124" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B125" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D134" s="3"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B135" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D135" s="3"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B136" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C138" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D138" s="3"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B139" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="C139" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="19" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D156" s="3"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D161" s="3"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C165" s="3"/>
       <c r="D165" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D166" s="3"/>
-    </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B167" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D167" s="3"/>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B168" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B178" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C176" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D176" s="3"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B177" s="3" t="s">
+      <c r="C178" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B179" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D177" s="3"/>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B178" s="3" t="s">
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B180" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D178" s="3"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B179" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B180" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B181" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B182" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B184" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D185" s="3"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D187" s="3"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E191" s="20"/>
       <c r="F191" s="21"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E192" s="24"/>
       <c r="F192" s="21"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D194" s="14"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D195" s="19"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" s="9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D210" s="3"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C216" s="3"/>
       <c r="D216" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D217" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B217" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D217" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B221" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C222" s="3"/>
       <c r="D222" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C223" s="3"/>
       <c r="D223" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C224" s="3"/>
       <c r="D224" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D225" s="18"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C228" s="3"/>
       <c r="D228" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C229" s="3"/>
       <c r="D229" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C231" s="3"/>
       <c r="D231" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C233" s="3"/>
       <c r="D233" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C234" s="3"/>
       <c r="D234" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B239" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D239" s="3"/>
-    </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B240" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="C240" s="3"/>
       <c r="D240" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B242" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C243" s="3"/>
       <c r="D243" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B244" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B245" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="23" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B247" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B248" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D249" s="3"/>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B250" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B252" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B253" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B254" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B255" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B256" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>19</v>
@@ -3593,26 +3595,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3626,7 +3628,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPI 11.3/Pramp, array element equal to its index, note in the plan
</commit_message>
<xml_diff>
--- a/Docs/EPI Interview Plan.xlsx
+++ b/Docs/EPI Interview Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="272">
   <si>
     <t>Задачи из EPI</t>
   </si>
@@ -1341,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
       <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
@@ -2284,7 +2284,7 @@
         <v>224</v>
       </c>
       <c r="C105" s="3"/>
-      <c r="D105" s="18" t="s">
+      <c r="D105" s="14" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3296,7 +3296,9 @@
       <c r="C225" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D225" s="18"/>
+      <c r="D225" s="18" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">

</xml_diff>